<commit_message>
23/11/22 - 14h23 - Exercice 1 fait
</commit_message>
<xml_diff>
--- a/Exercices/01 - Persistance des données/03 - Développer des composants/Exercices/Rangement pièces/Rangement de pièces.xlsx
+++ b/Exercices/01 - Persistance des données/03 - Développer des composants/Exercices/Rangement pièces/Rangement de pièces.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git\AFPA_CDA\Exercices\01 - Persistance des données\03 - Développer des composants\Exercices\Rangement pièces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F44ECBF5-86B2-400E-9FAB-44E953FB1882}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5CAD4E3-C74A-4978-ABF4-6D0D936AEABC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -550,8 +550,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="N15" sqref="N15"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="J3" sqref="J3:J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>